<commit_message>
New TC's for first project
</commit_message>
<xml_diff>
--- a/User Story Password Recovery/Login page TC's.xlsx
+++ b/User Story Password Recovery/Login page TC's.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Games\3mk\Manual Testing\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Games\3mk\Manual Testing\User Story Password Recovery\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEC61184-FDBA-4EE8-A33C-13B997B0CB9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9CAF90C-73F9-4385-8C52-4D754E2636D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{F74DBE0C-CFD5-4B1C-8808-1CA5DCC5CC54}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="45">
   <si>
     <t>TEST ID:</t>
   </si>
@@ -151,6 +151,42 @@
   </si>
   <si>
     <t>User should be able to log in using the new password</t>
+  </si>
+  <si>
+    <t>Verify error message appear for non-existing email</t>
+  </si>
+  <si>
+    <t>User on password recovery page</t>
+  </si>
+  <si>
+    <t>1-Navigate to login page
+2-Click on forgot password link
+3-Enter non-existing email
+4-Click on "Password recovery" button</t>
+  </si>
+  <si>
+    <t>1-An error message shall appear
+2-No email will be sent</t>
+  </si>
+  <si>
+    <t>Verify error message for expired password reset link</t>
+  </si>
+  <si>
+    <t>1-Navigate to login page
+2-Click on forgot 
+password link
+3-Wait for 24 Hour
+4-Click on "Password recovery" button</t>
+  </si>
+  <si>
+    <t>Verify error message for inequality new password and it's confirmation</t>
+  </si>
+  <si>
+    <t>1-Enter a new password 
+2-Enter a different password at the "confirm password" field</t>
+  </si>
+  <si>
+    <t>An error message shall appear</t>
   </si>
 </sst>
 </file>
@@ -552,50 +588,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77F66CEC-8F48-46EE-A4BF-DF2FB9D1A67B}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="96" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="21" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="22.88671875" customWidth="1"/>
-    <col min="2" max="2" width="24" customWidth="1"/>
-    <col min="3" max="3" width="10.6640625" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" customWidth="1"/>
-    <col min="5" max="5" width="25.109375" customWidth="1"/>
-    <col min="6" max="6" width="22.88671875" customWidth="1"/>
-    <col min="7" max="8" width="29.33203125" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
+    <col min="1" max="1" width="22.88671875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20" customWidth="1"/>
+    <col min="4" max="4" width="20.109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="25.109375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="22.88671875" style="3" customWidth="1"/>
+    <col min="7" max="8" width="29.33203125" style="3" customWidth="1"/>
+    <col min="9" max="9" width="17.88671875" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="70.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:9" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="I1" s="3" t="s">
         <v>6</v>
       </c>
     </row>
@@ -613,12 +649,9 @@
       <c r="E2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="F2" s="3"/>
       <c r="G2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="1"/>
-      <c r="I2" s="1"/>
     </row>
     <row r="3" spans="1:9" ht="84" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -634,12 +667,9 @@
       <c r="E3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3"/>
       <c r="G3" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1"/>
     </row>
     <row r="4" spans="1:9" ht="126" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -655,12 +685,9 @@
       <c r="E4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="3"/>
       <c r="G4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H4" s="1"/>
-      <c r="I4" s="1"/>
     </row>
     <row r="5" spans="1:9" ht="105" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -676,12 +703,9 @@
       <c r="E5" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="F5" s="3"/>
       <c r="G5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="H5" s="1"/>
-      <c r="I5" s="1"/>
     </row>
     <row r="6" spans="1:9" ht="84" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -697,12 +721,9 @@
       <c r="E6" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="H6" s="1"/>
-      <c r="I6" s="1"/>
     </row>
     <row r="7" spans="1:9" ht="126" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -718,12 +739,9 @@
       <c r="E7" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F7" s="3"/>
       <c r="G7" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="84" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -739,12 +757,61 @@
       <c r="E8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="F8" s="3"/>
       <c r="G8" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" ht="189" x14ac:dyDescent="0.3">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="168" x14ac:dyDescent="0.3">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="126" x14ac:dyDescent="0.3">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>